<commit_message>
Updates to Saltmarsh Map
Various updates to html styling.
Added new locations to data.xlsx.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucanSinclair\OneDrive - Earthwatch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucanSinclair\OneDrive - Earthwatch\Desktop\Code\Earthwatch_Code\Saltmarsh-Savers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F64BD90-0CA9-4972-BF06-A87B146503CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BA2F4B-1B50-48CE-AC93-98FBAE2A184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{EDC8C2C9-AF13-4847-9081-A01FE46671A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Machans Beach (Silver Site)" sheetId="1" r:id="rId1"/>
-    <sheet name="AFP Site" sheetId="2" r:id="rId2"/>
+    <sheet name="Machans Beach (Dump Site)" sheetId="3" r:id="rId2"/>
+    <sheet name="AFP Site" sheetId="2" r:id="rId3"/>
+    <sheet name="Jack Barnes Site" sheetId="4" r:id="rId4"/>
+    <sheet name="Thomatis (Site A)" sheetId="5" r:id="rId5"/>
+    <sheet name="Thomatis (Site B)" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="67">
   <si>
     <t>Threat</t>
   </si>
@@ -226,13 +230,22 @@
   </si>
   <si>
     <t>AFP Site</t>
+  </si>
+  <si>
+    <t>Jack Barnes Site</t>
+  </si>
+  <si>
+    <t>Thomatis (Site A)</t>
+  </si>
+  <si>
+    <t>Thomatis (site B)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -380,8 +393,24 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -561,8 +590,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -686,6 +721,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -731,13 +784,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1115,20 +1177,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9722E1D5-4268-4CFB-95A7-B673FD76448D}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E23"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="22.1796875" customWidth="1"/>
     <col min="2" max="2" width="17.7265625" customWidth="1"/>
     <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="7" max="7" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" customWidth="1"/>
+    <col min="4" max="4" width="28.453125" customWidth="1"/>
+    <col min="5" max="5" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" customWidth="1"/>
+    <col min="9" max="9" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,7 +1223,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1186,7 +1252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1197,16 +1263,16 @@
         <v>9.4072164950000001</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3">
-        <v>1.4878048779999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.6829268289999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1226,7 +1292,7 @@
         <v>2.5121951220000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1237,16 +1303,16 @@
         <v>6.25</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5">
-        <v>3.6829268289999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.292682927</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1257,16 +1323,16 @@
         <v>5.992268041</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6">
-        <v>2.292682927</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.4878048779999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1286,7 +1352,7 @@
         <v>2.6829268289999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1306,7 +1372,7 @@
         <v>3.414634146</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1326,7 +1392,7 @@
         <v>3.8780487799999999</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1346,7 +1412,7 @@
         <v>3.585365854</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1366,7 +1432,7 @@
         <v>1.7804878049999999</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1386,7 +1452,7 @@
         <v>1.195121951</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1406,7 +1472,7 @@
         <v>2.6585365849999998</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1426,7 +1492,7 @@
         <v>3.7317073170000001</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -1446,7 +1512,7 @@
         <v>2.414634146</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>40</v>
       </c>
@@ -1466,7 +1532,7 @@
         <v>2.9512195120000002</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1486,7 +1552,7 @@
         <v>3.292682927</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1506,7 +1572,7 @@
         <v>3.8292682930000002</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -1526,7 +1592,7 @@
         <v>3.4878048779999999</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1546,7 +1612,7 @@
         <v>1.243902439</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -1566,7 +1632,7 @@
         <v>3.414634146</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -1586,7 +1652,7 @@
         <v>3.6341463410000001</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1606,7 +1672,7 @@
         <v>3.5609756099999998</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1615,6 +1681,516 @@
       </c>
       <c r="C24">
         <v>0.77319587599999995</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D2:F6">
+    <sortCondition descending="1" ref="F2:F6"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F1C509-2F6E-4297-954C-B4FD037FDF3D}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.5">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>4.4858870967741939</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>5.1653660349312522</v>
+      </c>
+      <c r="G2" s="9">
+        <v>-16.858889000000001</v>
+      </c>
+      <c r="H2" s="7">
+        <v>145.733889</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>1.2096774193548387</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>3.8647342995169081</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.5">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0.90725806451612911</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>3.2701597918989216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.5">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0.30241935483870969</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>3.0471943515421773</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.5">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>5.5369751021924927</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.5">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>4.737903225806452</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>4.3849869936826451</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.5">
+      <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>4.0826612903225801</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>4.3106651802303979</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.5">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>7.8125</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>4.4593088071348941</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.5">
+      <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>1.2600806451612905</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>5.0538833147528788</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.5">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>7.0564516129032251</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>3.8647342995169081</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.5">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>3.7298387096774195</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>3.1586770717205495</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.5">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8.2157258064516139</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>5.2025269416573767</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.5">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>5.5947580645161299</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>5.5369751021924936</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.5">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>3.377016129032258</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15">
+        <v>4.9424005945745071</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.5">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>4.334677419354839</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>4.7565960609438864</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.5">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>6.0483870967741931</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>5.9457450761798576</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.5">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>4.838709677419355</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <v>5.5369751021924936</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.5">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.9717741935483861</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>5.4254923820141201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.5">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>8.11491935483871</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20">
+        <v>3.6789297658862874</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.5">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>2.1673387096774195</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21">
+        <v>3.6046079524340393</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.5">
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>4.8387096774193541</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>3.6417688591601634</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>4.737903225806452</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23">
+        <v>5.6112969156447408</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.5">
+      <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>3.1754032258064515</v>
       </c>
     </row>
   </sheetData>
@@ -1622,18 +2198,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9032AAA6-CDEB-4ECA-BC3D-9AB05617C8E9}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F23"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="24.453125" customWidth="1"/>
     <col min="2" max="2" width="21.54296875" customWidth="1"/>
+    <col min="3" max="3" width="20.54296875" customWidth="1"/>
     <col min="4" max="4" width="16.6328125" customWidth="1"/>
     <col min="5" max="5" width="17.1796875" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -1641,7 +2218,7 @@
     <col min="8" max="8" width="11.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1670,8 +2247,519 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="15.5">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>14.202561117578579</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>4.0358744394618826</v>
+      </c>
+      <c r="G2">
+        <v>-16.89546</v>
+      </c>
+      <c r="H2">
+        <v>145.7559</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>10.942956926658905</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>2.7902341803687092</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.5">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>10.128055878928986</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>4.5341305430991508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.5">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>9.6623981373690349</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0.29895366218236163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.5">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>6.7520372526193251</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>3.6372695565520661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.5">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>4.8894062863795105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>2.9895366218236168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.5">
+      <c r="A8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>3.0267753201396976</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>5.2815146985550561</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.5">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>2.2118742724097791</v>
+      </c>
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>5.0323866467364216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.5">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1.8626309662398137</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>3.3881415047334329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.5">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>1.7462165308498252</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>5.6302939711011444</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.5">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>1.280558789289872</v>
+      </c>
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>5.2316890881913292</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.5">
+      <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>0.69848661233993015</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>4.3846537120079718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.5">
+      <c r="A14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>0.58207217694994184</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>6.9257598405580447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.5">
+      <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15">
+        <v>4.4843049327354247</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.5">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>3.388141504733432</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.5">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>4.5839561534628794</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.5">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18">
+        <v>13.154831199068685</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <v>3.7867463876432481</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.5">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19">
+        <v>10.593713620488941</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>4.4843049327354247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.5">
+      <c r="A20" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>3.0267753201396972</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20">
+        <v>2.5909317389138007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.5">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>2.2118742724097791</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21">
+        <v>7.9720976581963114</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.5">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>1.5133876600698488</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>6.3278525161933219</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.5">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>0.93131548311990686</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23">
+        <v>8.2212257100149451</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.5">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>0.58207217694994184</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A18:C24">
+    <sortCondition descending="1" ref="C18:C24"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A37732-9494-4BA2-8F38-96E03CDFAC84}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.5">
+      <c r="A2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1680,27 +2768,27 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2">
-        <v>4.0358744394618826</v>
+        <v>5.924453280318092</v>
       </c>
       <c r="G2">
-        <v>-16.89546</v>
+        <v>-16.88336</v>
       </c>
       <c r="H2">
-        <v>145.7559</v>
+        <v>145.7611</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5">
+      <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1709,38 +2797,38 @@
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3">
-        <v>2.7902341803687092</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+        <v>2.7037773359840962</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.5">
+      <c r="A4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.58207217694994184</v>
-      </c>
-      <c r="D4" t="s">
+        <v>0.49751243781094528</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
       </c>
       <c r="F4">
-        <v>4.5341305430991508</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+        <v>5.7256461232604385</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.5">
+      <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1749,385 +2837,1399 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5">
-        <v>0.29895366218236163</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.5">
+      <c r="A6" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6">
-        <v>0.69848661233993015</v>
-      </c>
-      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6">
-        <v>3.6372695565520661</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+        <v>3.3001988071570585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.5">
+      <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7">
-        <v>4.8894062863795105</v>
-      </c>
-      <c r="D7" t="s">
+        <v>1.9071310116086235</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>22</v>
       </c>
       <c r="F7">
-        <v>2.9895366218236168</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+        <v>3.2206759443339963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.5">
+      <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C8">
-        <v>3.0267753201396972</v>
-      </c>
-      <c r="D8" t="s">
+        <v>1.4925373134328357</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E8" t="s">
         <v>22</v>
       </c>
       <c r="F8">
-        <v>5.2815146985550561</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+        <v>4.890656063618291</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.5">
+      <c r="A9" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C9">
-        <v>2.2118742724097791</v>
-      </c>
-      <c r="D9" t="s">
+        <v>1.3266998341625207</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>26</v>
       </c>
       <c r="E9" t="s">
         <v>22</v>
       </c>
       <c r="F9">
-        <v>5.0323866467364216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+        <v>6.0437375745526856</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.5">
+      <c r="A10" s="4" t="s">
         <v>60</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C10">
-        <v>0.58207217694994184</v>
-      </c>
-      <c r="D10" t="s">
+        <v>0.49751243781094528</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="E10" t="s">
         <v>29</v>
       </c>
       <c r="F10">
-        <v>3.3881415047334329</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+        <v>4.2544731610337978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.5">
+      <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C11">
-        <v>3.0267753201396976</v>
-      </c>
-      <c r="D11" t="s">
+        <v>6.8822553897180772</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>31</v>
       </c>
       <c r="E11" t="s">
         <v>29</v>
       </c>
       <c r="F11">
-        <v>5.6302939711011444</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+        <v>0.11928429423459246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.5">
+      <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C12">
-        <v>2.2118742724097791</v>
-      </c>
-      <c r="D12" t="s">
+        <v>5.9701492537313428</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>29</v>
       </c>
       <c r="F12">
-        <v>5.2316890881913292</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+        <v>3.9761431411530825</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.5">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13">
-        <v>1.8626309662398137</v>
-      </c>
-      <c r="D13" t="s">
+        <v>1.2437810945273633</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>35</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
       <c r="F13">
-        <v>4.3846537120079718</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+        <v>3.1013916500994045</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.5">
+      <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C14">
-        <v>10.942956926658905</v>
-      </c>
-      <c r="D14" t="s">
+        <v>9.8673300165837468</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>37</v>
       </c>
       <c r="E14" t="s">
         <v>29</v>
       </c>
       <c r="F14">
-        <v>6.9257598405580447</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+        <v>5.3280318091451306</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.5">
+      <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C15">
-        <v>1.280558789289872</v>
-      </c>
-      <c r="D15" t="s">
+        <v>3.5655058043117749</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>39</v>
       </c>
       <c r="E15" t="s">
         <v>29</v>
       </c>
       <c r="F15">
-        <v>4.4843049327354247</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+        <v>5.3280318091451297</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.5">
+      <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C16">
-        <v>6.7520372526193251</v>
-      </c>
-      <c r="D16" t="s">
+        <v>6.7993366500829193</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>41</v>
       </c>
       <c r="E16" t="s">
         <v>42</v>
       </c>
       <c r="F16">
-        <v>3.388141504733432</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+        <v>3.2604373757455276</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.5">
+      <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C17">
-        <v>9.6623981373690349</v>
-      </c>
-      <c r="D17" t="s">
+        <v>11.194029850746269</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E17" t="s">
         <v>42</v>
       </c>
       <c r="F17">
-        <v>4.5839561534628794</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+        <v>4.9701789264413527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.5">
+      <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C18">
-        <v>10.128055878928986</v>
-      </c>
-      <c r="D18" t="s">
+        <v>8.7064676616915406</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>47</v>
       </c>
       <c r="E18" t="s">
         <v>42</v>
       </c>
       <c r="F18">
-        <v>3.7867463876432481</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+        <v>4.3339960238568596</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.5">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19">
-        <v>14.202561117578579</v>
-      </c>
-      <c r="D19" t="s">
+        <v>14.2620232172471</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>49</v>
       </c>
       <c r="E19" t="s">
         <v>42</v>
       </c>
       <c r="F19">
-        <v>4.4843049327354247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+        <v>5.2485089463220689</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.5">
+      <c r="A20" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C20">
-        <v>13.154831199068685</v>
-      </c>
-      <c r="D20" t="s">
+        <v>12.85240464344942</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>51</v>
       </c>
       <c r="E20" t="s">
         <v>52</v>
       </c>
       <c r="F20">
-        <v>2.5909317389138007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+        <v>5.6461232604373768</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.5">
+      <c r="A21" s="4" t="s">
         <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C21">
-        <v>1.5133876600698488</v>
-      </c>
-      <c r="D21" t="s">
+        <v>0.49751243781094528</v>
+      </c>
+      <c r="D21" s="7" t="s">
         <v>54</v>
       </c>
       <c r="E21" t="s">
         <v>52</v>
       </c>
       <c r="F21">
-        <v>7.9720976581963114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+        <v>8.1510934393638177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.5">
+      <c r="A22" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C22">
-        <v>10.593713620488941</v>
-      </c>
-      <c r="D22" t="s">
+        <v>11.442786069651742</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>56</v>
       </c>
       <c r="E22" t="s">
         <v>57</v>
       </c>
       <c r="F22">
-        <v>6.3278525161933219</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+        <v>6.3220675944334008</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23">
-        <v>1.7462165308498252</v>
-      </c>
-      <c r="D23" t="s">
+        <v>0.99502487562189057</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>59</v>
       </c>
       <c r="E23" t="s">
         <v>57</v>
       </c>
       <c r="F23">
-        <v>8.2212257100149451</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+        <v>8.1510934393638177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.5">
+      <c r="A24" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C24">
-        <v>0.93131548311990686</v>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F84A2B-CB62-41C5-91B0-5634E1251A98}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.5">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>3.1478358628442948</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>4.8941542046999418</v>
+      </c>
+      <c r="G2" s="11">
+        <v>-16.837530000000001</v>
+      </c>
+      <c r="H2" s="11">
+        <v>145.72653</v>
+      </c>
+      <c r="I2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>2.4859195960380656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.5">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>3.8648281219654299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.5">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>2.1169159060011653</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.5">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>5.0689454262963674</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.5">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3.0916245081506468</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>6.234220236939211</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.5">
+      <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>3.9910061832490156</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>2.8355020392309185</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.5">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>2.2484541877459248</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>5.8652165469023103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.5">
+      <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>9.4435075885328832</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>5.4379491163332672</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.5">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>1.1242270938729624</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>6.7974363954165851</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.5">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0.78695896571107371</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>1.5536997475237908</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.5">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>8.4879145587408686</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>2.15575839968926</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.5">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>3.9910061832490165</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>3.2821907166440081</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.5">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>2.6981450252951094</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15">
+        <v>4.7387842299475622</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.5">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>3.7099494097807759</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>3.1462419887356763</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.5">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>9.6683530073074753</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>4.0590405904059041</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.5">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <v>6.6614876675082524</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.5">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>8.4317032040472171</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>6.8557001359487266</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.5">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>8.8813940415964012</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20">
+        <v>2.6218683239463969</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.5">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>6.5767284991568298</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21">
+        <v>7.0499126043892009</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.5">
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>11.410905002810566</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>5.4573703631773158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>11.523327712197863</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23">
+        <v>6.816857642260632</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.5">
+      <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>0.78695896571107371</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9047EB6-D702-48A6-8501-7AF99B0EA744}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="9" width="22.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.5">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>1.7266187050359711</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>5.477277237547133</v>
+      </c>
+      <c r="G2" s="11">
+        <v>-16.840209999999999</v>
+      </c>
+      <c r="H2" s="11">
+        <v>145.72797</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>2.6989482040087323</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.5">
+      <c r="A4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1.1510791366906474</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>4.5643976979559433</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.5">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>0.67146282973621096</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5">
+        <v>0.97241516173843989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.5">
+      <c r="A6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>0.67146282973621096</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>5.9734074221075604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.5">
+      <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>3.4052757793764994</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7">
+        <v>7.005358205993252</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.5">
+      <c r="A8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>1.3429256594724219</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>4.365945624131772</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.5">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>2.1103117505995201</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9">
+        <v>6.886286961698751</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.5">
+      <c r="A10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>2.014388489208633</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10">
+        <v>6.6878348878745779</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.5">
+      <c r="A11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>1.1510791366906474</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11">
+        <v>5.8741813851954765</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.5">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>0.67146282973621096</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12">
+        <v>1.9448303234768798</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.5">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>12.0863309352518</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.5">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>3.1654676258992804</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14">
+        <v>5.6161936892240538</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.5">
+      <c r="A15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>2.877697841726619</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15">
+        <v>4.2071839650724359</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.5">
+      <c r="A16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>4.2206235011990412</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>2.818019448303235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15.5">
+      <c r="A17" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>9.4964028776978413</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>3.0760071442746577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15.5">
+      <c r="A18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>1.5347721822541966</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18">
+        <v>4.8819210160746191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.5">
+      <c r="A19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>12.326139088729017</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19">
+        <v>5.4772772375471321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15.5">
+      <c r="A20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20">
+        <v>14.196642685851321</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20">
+        <v>1.6273070053582059</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.5">
+      <c r="A21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>7.1942446043165447</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21">
+        <v>6.9855129986108349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.5">
+      <c r="A22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>7.1942446043165464</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22">
+        <v>7.045048620758088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="16" thickBot="1">
+      <c r="A23" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>10.023980815347722</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23">
+        <v>5.8146457630482242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.5">
+      <c r="A24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>0.76738609112709832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed threat text to climate and human in data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucanSinclair\OneDrive - Earthwatch\Desktop\Code\Earthwatch_Code\Saltmarsh-Savers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81BA2F4B-1B50-48CE-AC93-98FBAE2A184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A6AA40-6A24-48B7-A16B-E8808A2FA9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{EDC8C2C9-AF13-4847-9081-A01FE46671A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" firstSheet="2" activeTab="5" xr2:uid="{EDC8C2C9-AF13-4847-9081-A01FE46671A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Machans Beach (Silver Site)" sheetId="1" r:id="rId1"/>
@@ -64,9 +64,6 @@
     <t xml:space="preserve">Buffer Zone condition </t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>Accessibility</t>
   </si>
   <si>
@@ -178,9 +175,6 @@
     <t>Coastal Squeeze</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Locally Iconic Species</t>
   </si>
   <si>
@@ -239,6 +233,12 @@
   </si>
   <si>
     <t>Thomatis (site B)</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>Climate</t>
   </si>
 </sst>
 </file>
@@ -788,9 +788,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -800,6 +797,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1177,8 +1177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9722E1D5-4268-4CFB-95A7-B673FD76448D}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1202,7 +1202,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1211,7 +1211,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1228,16 +1228,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C2">
         <v>10.76030928</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>3.804878049</v>
@@ -1249,24 +1249,24 @@
         <v>145.734722</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>9.4072164950000001</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>3.6829268289999999</v>
@@ -1274,19 +1274,19 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C4">
         <v>6.3788659790000004</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>2.5121951220000001</v>
@@ -1294,19 +1294,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C5">
         <v>6.25</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>2.292682927</v>
@@ -1314,19 +1314,19 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C6">
         <v>5.992268041</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>1.4878048779999999</v>
@@ -1334,19 +1334,19 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C7">
         <v>5.1546391749999998</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>2.6829268289999999</v>
@@ -1354,19 +1354,19 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>4.6391752579999999</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>3.414634146</v>
@@ -1374,19 +1374,19 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>4.1881443300000001</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>3.8780487799999999</v>
@@ -1394,19 +1394,19 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>4.1237113399999998</v>
       </c>
       <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>3.585365854</v>
@@ -1414,19 +1414,19 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C11">
         <v>3.7371134019999999</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>1.7804878049999999</v>
@@ -1434,19 +1434,19 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C12">
         <v>2.7706185570000001</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>1.195121951</v>
@@ -1454,19 +1454,19 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C13">
         <v>1.4175257729999999</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>2.6585365849999998</v>
@@ -1474,19 +1474,19 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C14">
         <v>0.57989690699999996</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>3.7317073170000001</v>
@@ -1494,19 +1494,19 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C15">
         <v>0.38659793799999997</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>2.414634146</v>
@@ -1514,19 +1514,19 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C16">
         <v>0.38659793799999997</v>
       </c>
       <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>2.9512195120000002</v>
@@ -1534,19 +1534,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>0.38659793799999997</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>3.292682927</v>
@@ -1554,19 +1554,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C18">
         <v>7.6675257730000004</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>3.8292682930000002</v>
@@ -1574,19 +1574,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C19">
         <v>7.6030927840000002</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>3.4878048779999999</v>
@@ -1594,19 +1594,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C20">
         <v>6.7010309279999998</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>1.243902439</v>
@@ -1614,19 +1614,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C21">
         <v>5.3479381439999996</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>3.414634146</v>
@@ -1634,19 +1634,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C22">
         <v>3.3505154639999999</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>3.6341463410000001</v>
@@ -1654,19 +1654,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C23">
         <v>1.9974226799999999</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>3.5609756099999998</v>
@@ -1674,10 +1674,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C24">
         <v>0.77319587599999995</v>
@@ -1695,13 +1695,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F1C509-2F6E-4297-954C-B4FD037FDF3D}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="9" width="22.26953125" customWidth="1"/>
+    <col min="1" max="1" width="22.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="3" max="9" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1">
@@ -1712,7 +1714,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1721,7 +1723,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1733,461 +1735,461 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C2">
         <v>4.4858870967741939</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>5.1653660349312522</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="8">
         <v>-16.858889000000001</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>145.733889</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.5">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C3">
         <v>1.2096774193548387</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>3.8647342995169081</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C4">
         <v>0.90725806451612911</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>3.2701597918989216</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5">
-      <c r="A5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
         <v>0.30241935483870969</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>17</v>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>3.0471943515421773</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.5">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>5.5369751021924927</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.5">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C7">
         <v>4.737903225806452</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>4.3849869936826451</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.5">
-      <c r="A8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C8">
         <v>4.0826612903225801</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>24</v>
+      <c r="D8" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>4.3106651802303979</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.5">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C9">
         <v>7.8125</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>26</v>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>4.4593088071348941</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.5">
-      <c r="A10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C10">
         <v>1.2600806451612905</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>5.0538833147528788</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.5">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C11">
         <v>7.0564516129032251</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>31</v>
+      <c r="D11" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>3.8647342995169081</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.5">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C12">
         <v>3.7298387096774195</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>33</v>
+      <c r="D12" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>3.1586770717205495</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.5">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C13">
         <v>8.2157258064516139</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>35</v>
+      <c r="D13" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>5.2025269416573767</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.5">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+    <row r="14" spans="1:9">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C14">
         <v>5.5947580645161299</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>37</v>
+      <c r="D14" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>5.5369751021924936</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.5">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C15">
         <v>3.377016129032258</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>39</v>
+      <c r="D15" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>4.9424005945745071</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.5">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C16">
         <v>4.334677419354839</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>4.7565960609438864</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C17">
         <v>6.0483870967741931</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>44</v>
+      <c r="D17" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>5.9457450761798576</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C18">
         <v>4.838709677419355</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>47</v>
+      <c r="D18" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>5.5369751021924936</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C19">
         <v>8.9717741935483861</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>49</v>
+      <c r="D19" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>5.4254923820141201</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C20">
         <v>8.11491935483871</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>51</v>
+      <c r="D20" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>3.6789297658862874</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C21">
         <v>2.1673387096774195</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>54</v>
+      <c r="D21" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>3.6046079524340393</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
         <v>4.8387096774193541</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>56</v>
+      <c r="D22" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>3.6417688591601634</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" thickBot="1">
-      <c r="A23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C23">
         <v>4.737903225806452</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>59</v>
+      <c r="D23" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>5.6112969156447408</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5">
-      <c r="A24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C24">
         <v>3.1754032258064515</v>
@@ -2202,8 +2204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9032AAA6-CDEB-4ECA-BC3D-9AB05617C8E9}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2226,7 +2228,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2235,7 +2237,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2247,21 +2249,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+      <c r="B2" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C2">
         <v>14.202561117578579</v>
       </c>
       <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>4.0358744394618826</v>
@@ -2273,435 +2275,435 @@
         <v>145.7559</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C3">
         <v>10.942956926658905</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2.7902341803687092</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C4">
         <v>10.128055878928986</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>4.5341305430991508</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
         <v>9.6623981373690349</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>0.29895366218236163</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.5">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C6">
         <v>6.7520372526193251</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>3.6372695565520661</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.5">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C7">
         <v>4.8894062863795105</v>
       </c>
       <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>2.9895366218236168</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.5">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C8">
         <v>3.0267753201396976</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>5.2815146985550561</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.5">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C9">
         <v>2.2118742724097791</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>5.0323866467364216</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.5">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C10">
         <v>1.8626309662398137</v>
       </c>
       <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>3.3881415047334329</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.5">
+    <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+        <v>26</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C11">
         <v>1.7462165308498252</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>5.6302939711011444</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.5">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C12">
         <v>1.280558789289872</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>5.2316890881913292</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.5">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C13">
         <v>0.69848661233993015</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>4.3846537120079718</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.5">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>35</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C14">
         <v>0.58207217694994184</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>6.9257598405580447</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.5">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>4.4843049327354247</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.5">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+        <v>37</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>3.388141504733432</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5">
+    <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>39</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>4.5839561534628794</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5">
+    <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C18">
         <v>13.154831199068685</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>3.7867463876432481</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5">
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C19">
         <v>10.593713620488941</v>
       </c>
       <c r="D19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>4.4843049327354247</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5">
+    <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C20">
         <v>3.0267753201396972</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>2.5909317389138007</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5">
+    <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C21">
         <v>2.2118742724097791</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>7.9720976581963114</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5">
+    <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>51</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
         <v>1.5133876600698488</v>
       </c>
       <c r="D22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>6.3278525161933219</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.5">
+    <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C23">
         <v>0.93131548311990686</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>8.2212257100149451</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5">
+    <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C24">
         <v>0.58207217694994184</v>
@@ -2719,7 +2721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A37732-9494-4BA2-8F38-96E03CDFAC84}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
@@ -2737,7 +2739,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -2746,7 +2748,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -2758,21 +2760,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>5.924453280318092</v>
@@ -2784,435 +2786,435 @@
         <v>145.7611</v>
       </c>
       <c r="I2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.5">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>13</v>
+      <c r="D3" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2.7037773359840962</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C4">
         <v>0.49751243781094528</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>5.7256461232604385</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5">
-      <c r="A5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>17</v>
+      <c r="D5" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.5">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>3.3001988071570585</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.5">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C7">
         <v>1.9071310116086235</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>3.2206759443339963</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.5">
-      <c r="A8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C8">
         <v>1.4925373134328357</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>24</v>
+      <c r="D8" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>4.890656063618291</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.5">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C9">
         <v>1.3266998341625207</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>26</v>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>6.0437375745526856</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.5">
-      <c r="A10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C10">
         <v>0.49751243781094528</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>4.2544731610337978</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.5">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C11">
         <v>6.8822553897180772</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>31</v>
+      <c r="D11" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>0.11928429423459246</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.5">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C12">
         <v>5.9701492537313428</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>33</v>
+      <c r="D12" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>3.9761431411530825</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.5">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C13">
         <v>1.2437810945273633</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>35</v>
+      <c r="D13" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>3.1013916500994045</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.5">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+    <row r="14" spans="1:9">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C14">
         <v>9.8673300165837468</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>37</v>
+      <c r="D14" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>5.3280318091451306</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.5">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C15">
         <v>3.5655058043117749</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>39</v>
+      <c r="D15" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>5.3280318091451297</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.5">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C16">
         <v>6.7993366500829193</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>3.2604373757455276</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C17">
         <v>11.194029850746269</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>44</v>
+      <c r="D17" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>4.9701789264413527</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C18">
         <v>8.7064676616915406</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>47</v>
+      <c r="D18" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>4.3339960238568596</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C19">
         <v>14.2620232172471</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>49</v>
+      <c r="D19" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>5.2485089463220689</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C20">
         <v>12.85240464344942</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>51</v>
+      <c r="D20" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>5.6461232604373768</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C21">
         <v>0.49751243781094528</v>
       </c>
-      <c r="D21" s="7" t="s">
-        <v>54</v>
+      <c r="D21" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>8.1510934393638177</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
         <v>11.442786069651742</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>56</v>
+      <c r="D22" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>6.3220675944334008</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" thickBot="1">
-      <c r="A23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C23">
         <v>0.99502487562189057</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>59</v>
+      <c r="D23" s="7" t="s">
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>8.1510934393638177</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5">
-      <c r="A24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -3228,7 +3230,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3244,7 +3246,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3253,7 +3255,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -3265,461 +3267,461 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C2">
         <v>3.1478358628442948</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>4.8941542046999418</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>-16.837530000000001</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>145.72653</v>
       </c>
       <c r="I2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.5">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2.4859195960380656</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>15</v>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>3.8648281219654299</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5">
-      <c r="A5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>2.1169159060011653</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.5">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>19</v>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>5.0689454262963674</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.5">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C7">
         <v>3.0916245081506468</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>6.234220236939211</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.5">
-      <c r="A8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C8">
         <v>3.9910061832490156</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>24</v>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>2.8355020392309185</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.5">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C9">
         <v>2.2484541877459248</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>26</v>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>5.8652165469023103</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.5">
-      <c r="A10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C10">
         <v>9.4435075885328832</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>5.4379491163332672</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.5">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C11">
         <v>1.1242270938729624</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>31</v>
+      <c r="D11" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>6.7974363954165851</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.5">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C12">
         <v>0.78695896571107371</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>33</v>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>1.5536997475237908</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.5">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C13">
         <v>8.4879145587408686</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>35</v>
+      <c r="D13" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>2.15575839968926</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.5">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+    <row r="14" spans="1:9">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C14">
         <v>3.9910061832490165</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>37</v>
+      <c r="D14" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>3.2821907166440081</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.5">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C15">
         <v>2.6981450252951094</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>39</v>
+      <c r="D15" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>4.7387842299475622</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.5">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C16">
         <v>3.7099494097807759</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>3.1462419887356763</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C17">
         <v>9.6683530073074753</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>44</v>
+      <c r="D17" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>4.0590405904059041</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>47</v>
+      <c r="D18" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>6.6614876675082524</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C19">
         <v>8.4317032040472171</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>49</v>
+      <c r="D19" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>6.8557001359487266</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C20">
         <v>8.8813940415964012</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>51</v>
+      <c r="D20" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>2.6218683239463969</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C21">
         <v>6.5767284991568298</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>54</v>
+      <c r="D21" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>7.0499126043892009</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
         <v>11.410905002810566</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>56</v>
+      <c r="D22" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>5.4573703631773158</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" thickBot="1">
-      <c r="A23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C23">
         <v>11.523327712197863</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>59</v>
+      <c r="D23" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>6.816857642260632</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5">
-      <c r="A24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C24">
         <v>0.78695896571107371</v>
@@ -3734,8 +3736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9047EB6-D702-48A6-8501-7AF99B0EA744}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3751,7 +3753,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -3760,7 +3762,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -3772,461 +3774,461 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.5">
-      <c r="A2" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C2">
         <v>1.7266187050359711</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
       </c>
       <c r="F2">
         <v>5.477277237547133</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="10">
         <v>-16.840209999999999</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="10">
         <v>145.72797</v>
       </c>
       <c r="I2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.5">
-      <c r="A3" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>13</v>
+      <c r="D3" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3">
         <v>2.6989482040087323</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.5">
-      <c r="A4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C4">
         <v>1.1510791366906474</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>15</v>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4">
         <v>4.5643976979559433</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.5">
-      <c r="A5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
+    <row r="5" spans="1:9">
+      <c r="A5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C5">
         <v>0.67146282973621096</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>17</v>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5">
         <v>0.97241516173843989</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.5">
-      <c r="A6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>8</v>
+    <row r="6" spans="1:9">
+      <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C6">
         <v>0.67146282973621096</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>19</v>
+      <c r="D6" s="10" t="s">
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6">
         <v>5.9734074221075604</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.5">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
+    <row r="7" spans="1:9">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C7">
         <v>3.4052757793764994</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
       </c>
       <c r="F7">
         <v>7.005358205993252</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.5">
-      <c r="A8" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>46</v>
+    <row r="8" spans="1:9">
+      <c r="A8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C8">
         <v>1.3429256594724219</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>24</v>
+      <c r="D8" s="10" t="s">
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8">
         <v>4.365945624131772</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.5">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:9">
+      <c r="A9" s="3" t="s">
         <v>46</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C9">
         <v>2.1103117505995201</v>
       </c>
-      <c r="D9" s="11" t="s">
-        <v>26</v>
+      <c r="D9" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9">
         <v>6.886286961698751</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.5">
-      <c r="A10" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>46</v>
+    <row r="10" spans="1:9">
+      <c r="A10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C10">
         <v>2.014388489208633</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
       <c r="F10">
         <v>6.6878348878745779</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.5">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>8</v>
+    <row r="11" spans="1:9">
+      <c r="A11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C11">
         <v>1.1510791366906474</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>31</v>
+      <c r="D11" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11">
         <v>5.8741813851954765</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.5">
-      <c r="A12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+    <row r="12" spans="1:9">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C12">
         <v>0.67146282973621096</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>33</v>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
         <v>1.9448303234768798</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.5">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+    <row r="13" spans="1:9">
+      <c r="A13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C13">
         <v>12.0863309352518</v>
       </c>
-      <c r="D13" s="11" t="s">
-        <v>35</v>
+      <c r="D13" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.5">
-      <c r="A14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>8</v>
+    <row r="14" spans="1:9">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C14">
         <v>3.1654676258992804</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>37</v>
+      <c r="D14" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14">
         <v>5.6161936892240538</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.5">
-      <c r="A15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
+    <row r="15" spans="1:9">
+      <c r="A15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C15">
         <v>2.877697841726619</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>39</v>
+      <c r="D15" s="10" t="s">
+        <v>38</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15">
         <v>4.2071839650724359</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.5">
-      <c r="A16" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>8</v>
+    <row r="16" spans="1:9">
+      <c r="A16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C16">
         <v>4.2206235011990412</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>2.818019448303235</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15.5">
-      <c r="A17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C17">
         <v>9.4964028776978413</v>
       </c>
-      <c r="D17" s="11" t="s">
-        <v>44</v>
+      <c r="D17" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17">
         <v>3.0760071442746577</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.5">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C18">
         <v>1.5347721822541966</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>47</v>
+      <c r="D18" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18">
         <v>4.8819210160746191</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15.5">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>8</v>
+      <c r="B19" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C19">
         <v>12.326139088729017</v>
       </c>
-      <c r="D19" s="11" t="s">
-        <v>49</v>
+      <c r="D19" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="E19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19">
         <v>5.4772772375471321</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.5">
-      <c r="A20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>46</v>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C20">
         <v>14.196642685851321</v>
       </c>
-      <c r="D20" s="11" t="s">
-        <v>51</v>
+      <c r="D20" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20">
         <v>1.6273070053582059</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.5">
-      <c r="A21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C21">
         <v>7.1942446043165447</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>54</v>
+      <c r="D21" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="E21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F21">
         <v>6.9855129986108349</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.5">
-      <c r="A22" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>46</v>
+    <row r="22" spans="1:6">
+      <c r="A22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
         <v>7.1942446043165464</v>
       </c>
-      <c r="D22" s="11" t="s">
-        <v>56</v>
+      <c r="D22" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F22">
         <v>7.045048620758088</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="16" thickBot="1">
-      <c r="A23" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
+    <row r="23" spans="1:6" ht="15" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>65</v>
       </c>
       <c r="C23">
         <v>10.023980815347722</v>
       </c>
-      <c r="D23" s="12" t="s">
-        <v>59</v>
+      <c r="D23" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="E23" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F23">
         <v>5.8146457630482242</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.5">
-      <c r="A24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>46</v>
+    <row r="24" spans="1:6">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>66</v>
       </c>
       <c r="C24">
         <v>0.76738609112709832</v>

</xml_diff>